<commit_message>
created Registration, Internal entry
</commit_message>
<xml_diff>
--- a/studentms_database_design.xlsx
+++ b/studentms_database_design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>student</t>
   </si>
@@ -117,13 +117,40 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>semester registration</t>
+  </si>
+  <si>
+    <t>internal attendance marks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user </t>
+  </si>
+  <si>
+    <t>receipt_no</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>registration form photo</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +158,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +193,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -216,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -237,6 +285,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -246,9 +297,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,30 +612,31 @@
   <dimension ref="A2:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.140625" bestFit="1" customWidth="1"/>
@@ -595,14 +648,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
       <c r="I2" s="9" t="s">
         <v>11</v>
       </c>
@@ -713,10 +766,13 @@
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="G6" s="12" t="s">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="14"/>
       <c r="U6">
         <v>1</v>
       </c>
@@ -739,10 +795,10 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="J8" s="14"/>
       <c r="U8">
         <v>3</v>
       </c>
@@ -751,6 +807,9 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>1</v>
       </c>
@@ -765,10 +824,10 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="3"/>
       <c r="U10">
         <v>5</v>
@@ -798,6 +857,27 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="M13" s="1" t="s">
         <v>1</v>
       </c>
@@ -815,6 +895,7 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
       <c r="O15" s="1" t="s">
         <v>1</v>
       </c>
@@ -828,6 +909,9 @@
       <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="O16">
         <v>1</v>
       </c>
@@ -838,7 +922,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="O17">
         <v>2</v>
       </c>
@@ -849,7 +936,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="O18">
         <v>3</v>
       </c>
@@ -860,9 +950,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>29</v>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="O19">
         <v>4</v>
@@ -874,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O20">
         <v>5</v>
       </c>
@@ -885,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="O21">
         <v>6</v>
       </c>
@@ -898,14 +988,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="I2:R2"/>
     <mergeCell ref="T4:AB4"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="O14:Q14"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="I2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>

</xml_diff>